<commit_message>
New code for hints files, in progress
</commit_message>
<xml_diff>
--- a/osiris/Documentation/Ping Failure Message Glossary.xlsx
+++ b/osiris/Documentation/Ping Failure Message Glossary.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\goorrob\Documents\GitHub\osiris\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7F05BDC-618F-4C32-BC67-D1595F7357DE}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF3C44F0-DDCF-4F79-9964-C80348EC3A0B}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="21255" yWindow="5850" windowWidth="13320" windowHeight="10845" xr2:uid="{A226AE24-A6A6-4452-B12A-847F8A89D7E9}"/>
+    <workbookView xWindow="5070" yWindow="5070" windowWidth="28800" windowHeight="15435" xr2:uid="{A226AE24-A6A6-4452-B12A-847F8A89D7E9}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="66">
   <si>
     <t>Message Number</t>
   </si>
@@ -226,6 +226,9 @@
   </si>
   <si>
     <t>Catastrophic crash not caught at analysis level</t>
+  </si>
+  <si>
+    <t>Mod pair used by multiple samples</t>
   </si>
 </sst>
 </file>
@@ -609,8 +612,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E696A1A8-6E12-4BA5-8D4E-21FCB21D7714}">
   <dimension ref="A1:D644"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
-      <selection activeCell="C67" sqref="C67"/>
+    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="C68" sqref="C68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1216,7 +1219,12 @@
       <c r="D67" s="6"/>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A68" s="5"/>
+      <c r="A68" s="5">
+        <v>651</v>
+      </c>
+      <c r="C68" t="s">
+        <v>65</v>
+      </c>
       <c r="D68" s="6"/>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
mods files working and extra print statements removed:  works for ILS and Ladder channels only
</commit_message>
<xml_diff>
--- a/osiris/Documentation/Ping Failure Message Glossary.xlsx
+++ b/osiris/Documentation/Ping Failure Message Glossary.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\goorrob\Documents\GitHub\osiris\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF3C44F0-DDCF-4F79-9964-C80348EC3A0B}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9ABCB3D6-CCA4-46D5-889C-9F9A9B01ABE0}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5070" yWindow="5070" windowWidth="28800" windowHeight="15435" xr2:uid="{A226AE24-A6A6-4452-B12A-847F8A89D7E9}"/>
+    <workbookView xWindow="8325" yWindow="4575" windowWidth="28800" windowHeight="15435" xr2:uid="{A226AE24-A6A6-4452-B12A-847F8A89D7E9}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="67">
   <si>
     <t>Message Number</t>
   </si>
@@ -229,6 +229,9 @@
   </si>
   <si>
     <t>Mod pair used by multiple samples</t>
+  </si>
+  <si>
+    <t>Sample pre-edited using mods file</t>
   </si>
 </sst>
 </file>
@@ -613,7 +616,7 @@
   <dimension ref="A1:D644"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="C68" sqref="C68"/>
+      <selection activeCell="C69" sqref="C69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1228,7 +1231,12 @@
       <c r="D68" s="6"/>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A69" s="5"/>
+      <c r="A69" s="5">
+        <v>652</v>
+      </c>
+      <c r="C69" t="s">
+        <v>66</v>
+      </c>
       <c r="D69" s="6"/>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>